<commit_message>
sn: update itas form
</commit_message>
<xml_diff>
--- a/LF/ITAS/sn_lf_itas_20305_3_dbs.xlsx
+++ b/LF/ITAS/sn_lf_itas_20305_3_dbs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\LF\ITAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3C9FE87-628E-4BDF-BA87-DE87CD44EE7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9F01992-5587-40A8-BF89-32C63A3C3864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -554,9 +554,6 @@
   </si>
   <si>
     <t>read_only</t>
-  </si>
-  <si>
-    <t>concat(${o_BarcodeID})</t>
   </si>
   <si>
     <t>image</t>
@@ -684,6 +681,9 @@
   </si>
   <si>
     <t>sn_lf_itas_20305_3_dbs_v3</t>
+  </si>
+  <si>
+    <t>if(${o_IDType} = 'Scanner', concat(${o_BarcodeID}), concat(${o_manual_code_id}))</t>
   </si>
 </sst>
 </file>
@@ -1525,11 +1525,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomRight" activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1770,7 +1770,7 @@
         <v>59</v>
       </c>
       <c r="B9" s="33" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C9" s="37" t="s">
         <v>117</v>
@@ -1950,7 +1950,7 @@
       </c>
       <c r="H16" s="23"/>
       <c r="I16" s="25" t="s">
-        <v>177</v>
+        <v>215</v>
       </c>
       <c r="J16" s="23" t="s">
         <v>16</v>
@@ -1964,13 +1964,13 @@
     </row>
     <row r="17" spans="1:13" s="10" customFormat="1">
       <c r="A17" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="B17" s="13" t="s">
         <v>181</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="C17" s="15" t="s">
         <v>182</v>
-      </c>
-      <c r="C17" s="15" t="s">
-        <v>183</v>
       </c>
       <c r="D17" s="17"/>
       <c r="E17" s="12"/>
@@ -1987,13 +1987,13 @@
     </row>
     <row r="18" spans="1:13" s="10" customFormat="1">
       <c r="A18" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="C18" s="15" t="s">
         <v>184</v>
-      </c>
-      <c r="B18" s="13" t="s">
-        <v>189</v>
-      </c>
-      <c r="C18" s="15" t="s">
-        <v>185</v>
       </c>
       <c r="D18" s="17"/>
       <c r="E18" s="12"/>
@@ -2016,10 +2016,10 @@
         <v>98</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E19" s="12"/>
       <c r="F19" s="12"/>
@@ -2066,7 +2066,7 @@
         <v>101</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D21" s="17"/>
       <c r="E21" s="12"/>
@@ -2085,20 +2085,20 @@
     </row>
     <row r="22" spans="1:13" s="10" customFormat="1" ht="31.5">
       <c r="A22" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="B22" s="13" t="s">
         <v>178</v>
       </c>
-      <c r="B22" s="13" t="s">
-        <v>179</v>
-      </c>
       <c r="C22" s="15" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D22" s="17"/>
       <c r="E22" s="12"/>
       <c r="F22" s="12"/>
       <c r="G22" s="17"/>
       <c r="H22" s="13" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="I22" s="13"/>
       <c r="J22" s="12" t="s">
@@ -2110,16 +2110,16 @@
     </row>
     <row r="23" spans="1:13" s="10" customFormat="1">
       <c r="A23" s="12" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D23" s="17" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E23" s="12"/>
       <c r="F23" s="12"/>
@@ -2164,7 +2164,7 @@
         <v>105</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D25" s="17"/>
       <c r="E25" s="12"/>
@@ -2187,16 +2187,16 @@
         <v>106</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D26" s="18" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E26" s="11"/>
       <c r="F26" s="11"/>
       <c r="G26" s="18"/>
       <c r="H26" s="13" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="I26" s="11"/>
       <c r="J26" s="12" t="s">
@@ -2214,7 +2214,7 @@
         <v>107</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D27" s="18"/>
       <c r="E27" s="11"/>
@@ -2239,7 +2239,7 @@
         <v>109</v>
       </c>
       <c r="C28" s="18" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D28" s="18"/>
       <c r="E28" s="11"/>
@@ -2258,20 +2258,20 @@
     </row>
     <row r="29" spans="1:13" s="10" customFormat="1" ht="31.5">
       <c r="A29" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D29" s="17"/>
       <c r="E29" s="12"/>
       <c r="F29" s="12"/>
       <c r="G29" s="17"/>
       <c r="H29" s="13" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I29" s="13"/>
       <c r="J29" s="12" t="s">
@@ -2283,16 +2283,16 @@
     </row>
     <row r="30" spans="1:13" s="10" customFormat="1">
       <c r="A30" s="12" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B30" s="13" t="s">
+        <v>190</v>
+      </c>
+      <c r="C30" s="15" t="s">
+        <v>201</v>
+      </c>
+      <c r="D30" s="18" t="s">
         <v>191</v>
-      </c>
-      <c r="C30" s="15" t="s">
-        <v>202</v>
-      </c>
-      <c r="D30" s="18" t="s">
-        <v>192</v>
       </c>
       <c r="E30" s="12"/>
       <c r="F30" s="12"/>
@@ -2320,7 +2320,7 @@
       <c r="G31" s="18"/>
       <c r="H31" s="12"/>
       <c r="I31" s="20" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J31" s="11"/>
       <c r="K31" s="11"/>
@@ -2371,7 +2371,7 @@
         <v>27</v>
       </c>
       <c r="C34" s="18" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D34" s="18"/>
       <c r="E34" s="11"/>
@@ -2450,7 +2450,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="B9:B14"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2565,7 +2565,7 @@
         <v>56</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C9" s="19" t="s">
         <v>43</v>
@@ -2576,7 +2576,7 @@
         <v>56</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C10" s="19" t="s">
         <v>44</v>
@@ -2587,7 +2587,7 @@
         <v>56</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C11" s="19" t="s">
         <v>45</v>
@@ -2598,7 +2598,7 @@
         <v>56</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C12" s="19" t="s">
         <v>46</v>
@@ -2609,10 +2609,10 @@
         <v>56</v>
       </c>
       <c r="B13" s="19" t="s">
+        <v>206</v>
+      </c>
+      <c r="C13" s="19" t="s">
         <v>207</v>
-      </c>
-      <c r="C13" s="19" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -2620,10 +2620,10 @@
         <v>56</v>
       </c>
       <c r="B14" s="19" t="s">
+        <v>208</v>
+      </c>
+      <c r="C14" s="19" t="s">
         <v>209</v>
-      </c>
-      <c r="C14" s="19" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -3865,7 +3865,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -3888,10 +3888,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="B2" t="s">
         <v>214</v>
-      </c>
-      <c r="B2" t="s">
-        <v>215</v>
       </c>
       <c r="C2" t="s">
         <v>52</v>

</xml_diff>